<commit_message>
newer plots or something??
</commit_message>
<xml_diff>
--- a/data/1000_automated_withplots.xlsx
+++ b/data/1000_automated_withplots.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Time</t>
   </si>
@@ -94,12 +94,18 @@
   <si>
     <t>alpha</t>
   </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>noise from avg (from constant csv)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -123,6 +129,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -141,21 +154,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3413,346 +3439,346 @@
                   <c:v>17.9882526397705</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.98262977600095</c:v>
+                  <c:v>17.98038063049313</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.98477935791012</c:v>
+                  <c:v>17.98496444702145</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17.99049091339106</c:v>
+                  <c:v>17.99283106231683</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18.02299356460568</c:v>
+                  <c:v>18.03669666976926</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.25388264656064</c:v>
+                  <c:v>18.3503492108917</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18.21487390995022</c:v>
+                  <c:v>18.22821038460537</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.26130753755566</c:v>
+                  <c:v>18.28388193099438</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18.32351055741308</c:v>
+                  <c:v>18.35516408338767</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>18.35567255318159</c:v>
+                  <c:v>18.37803340928137</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18.46071896702045</c:v>
+                  <c:v>18.50944578938592</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>18.53992502763862</c:v>
+                  <c:v>18.58622549859554</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>18.79964848794036</c:v>
+                  <c:v>18.91742801334813</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18.81201563496138</c:v>
+                  <c:v>18.85229635139212</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>18.85675244638694</c:v>
+                  <c:v>18.88673138588639</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.95845606480722</c:v>
+                  <c:v>19.00813119402517</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19.11419297533571</c:v>
+                  <c:v>19.19139027831249</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.25369167962341</c:v>
+                  <c:v>19.33265035223152</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19.41259813625945</c:v>
+                  <c:v>19.49984832069631</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19.76298451582258</c:v>
+                  <c:v>19.92931412297888</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19.81818831046254</c:v>
+                  <c:v>19.89016871046541</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.84311324397637</c:v>
+                  <c:v>19.87467733738276</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19.95702186246668</c:v>
+                  <c:v>20.01205453788473</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20.04539211104289</c:v>
+                  <c:v>20.0972500130988</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>20.1049304381508</c:v>
+                  <c:v>20.14430313961073</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>20.13190247493475</c:v>
+                  <c:v>20.15450310008631</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>20.30372799375397</c:v>
+                  <c:v>20.37923838882713</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>20.49322981108594</c:v>
+                  <c:v>20.59168365654067</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20.47512766952002</c:v>
+                  <c:v>20.49742296653007</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.54139588889816</c:v>
+                  <c:v>20.57459176575243</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>20.63478218822348</c:v>
+                  <c:v>20.68209547100989</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>20.70179623022009</c:v>
+                  <c:v>20.74279583185466</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>20.7353032512184</c:v>
+                  <c:v>20.76100594010809</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>20.7627722463367</c:v>
+                  <c:v>20.78147065105093</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>21.05844815777525</c:v>
+                  <c:v>21.18232804376494</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.96754328512537</c:v>
+                  <c:v>20.96834530186233</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>20.92623265635659</c:v>
+                  <c:v>20.90994900987016</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>20.90557734197219</c:v>
+                  <c:v>20.8924301222725</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>21.0073846182517</c:v>
+                  <c:v>21.0441633628536</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>21.09755865739245</c:v>
+                  <c:v>21.14466189642932</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>21.16162951790518</c:v>
+                  <c:v>21.20138883382133</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>21.51795236271234</c:v>
+                  <c:v>21.67240929541005</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>21.53714104494257</c:v>
+                  <c:v>21.59115359764397</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>21.56386528412898</c:v>
+                  <c:v>21.59075874561398</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>21.66471367081204</c:v>
+                  <c:v>21.71312106393076</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>21.77425899605052</c:v>
+                  <c:v>21.83259934408153</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>21.84157056858186</c:v>
+                  <c:v>21.8859973020037</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>22.02165350938858</c:v>
+                  <c:v>22.10701470573782</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>22.17003505242374</c:v>
+                  <c:v>22.25499602854257</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>22.72863610989107</c:v>
+                  <c:v>22.97756482571365</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>22.73085705641034</c:v>
+                  <c:v>22.80642404976481</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>22.87008341254352</c:v>
+                  <c:v>22.94844405300314</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>22.99763516635476</c:v>
+                  <c:v>23.07216406001714</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>23.07621016130238</c:v>
+                  <c:v>23.12999882738014</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>23.11196811013114</c:v>
+                  <c:v>23.14240788948597</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>23.12420896198692</c:v>
+                  <c:v>23.13823723653568</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>23.36178900552956</c:v>
+                  <c:v>23.46102950531125</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>23.68301070607288</c:v>
+                  <c:v>23.84127153622471</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>23.67949706751394</c:v>
+                  <c:v>23.72556986113592</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>23.67321410992882</c:v>
+                  <c:v>23.68452276498137</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>23.66630561758646</c:v>
+                  <c:v>23.66693481716528</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>23.76431945765793</c:v>
+                  <c:v>23.80371375356017</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>23.91983177167561</c:v>
+                  <c:v>23.99385498605336</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>23.98411918631385</c:v>
+                  <c:v>24.03204111648247</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>24.40011775966083</c:v>
+                  <c:v>24.5808937680502</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>24.33736700055791</c:v>
+                  <c:v>24.36649949943356</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>24.33948275565</c:v>
+                  <c:v>24.34906880734954</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>24.4977462148611</c:v>
+                  <c:v>24.5639274140554</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>24.60940014600475</c:v>
+                  <c:v>24.6739160782205</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>24.63952940344668</c:v>
+                  <c:v>24.67093588608817</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>24.65544852435514</c:v>
+                  <c:v>24.67123811751097</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>24.67367057412822</c:v>
+                  <c:v>24.6856962719842</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>25.35163059040881</c:v>
+                  <c:v>25.62642230627784</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>25.3042990674822</c:v>
+                  <c:v>25.36780397307227</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>25.2925618643685</c:v>
+                  <c:v>25.30691845480004</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>25.4842049357853</c:v>
+                  <c:v>25.56516914148148</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>25.63720496880815</c:v>
+                  <c:v>25.72269424372615</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>25.72738448971413</c:v>
+                  <c:v>25.78910308055191</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>25.76172157224961</c:v>
+                  <c:v>25.79397198251515</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>25.9177794262615</c:v>
+                  <c:v>25.98987769094592</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>26.69324850066735</c:v>
+                  <c:v>27.02506560983502</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>26.69910227767743</c:v>
+                  <c:v>26.80098892123176</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>26.91043847556966</c:v>
+                  <c:v>27.02553894779285</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>27.07205006359048</c:v>
+                  <c:v>27.17122484046577</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>27.30113504766434</c:v>
+                  <c:v>27.42252147435647</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>27.57013558566077</c:v>
+                  <c:v>27.71415172886698</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>27.71692204087724</c:v>
+                  <c:v>27.81884146592569</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>27.78171217247717</c:v>
+                  <c:v>27.83820405263167</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>27.87094241283769</c:v>
+                  <c:v>27.92358207302824</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>27.97184053014929</c:v>
+                  <c:v>28.0279916751311</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>28.3236344603261</c:v>
+                  <c:v>28.48119737589136</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>28.56026331323185</c:v>
+                  <c:v>28.70218372906373</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>28.68673260876432</c:v>
+                  <c:v>28.77989645172688</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>28.71877733801251</c:v>
+                  <c:v>28.75954438260055</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>28.69844373034655</c:v>
+                  <c:v>28.70254040065659</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>28.83538405084218</c:v>
+                  <c:v>28.89138918013343</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>29.53634913754264</c:v>
+                  <c:v>29.8335367110102</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>29.70161382353202</c:v>
+                  <c:v>29.85687596996804</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>29.82074518996421</c:v>
+                  <c:v>29.91497638046789</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>29.8879478971061</c:v>
+                  <c:v>29.94309833711397</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>29.93532602985185</c:v>
+                  <c:v>29.97082241495251</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>29.89050694803137</c:v>
+                  <c:v>29.88322823083338</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>30.06233893086379</c:v>
+                  <c:v>30.12888810883735</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>30.31767325724094</c:v>
+                  <c:v>30.43977174118388</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>30.75518729848127</c:v>
+                  <c:v>30.96682246016028</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>30.85619033655749</c:v>
+                  <c:v>30.96008210029168</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>30.9202063743334</c:v>
+                  <c:v>30.97698031856401</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>30.96915927847525</c:v>
+                  <c:v>31.00577262340117</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>31.26181753138847</c:v>
+                  <c:v>31.38986483603154</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>31.57699851026209</c:v>
+                  <c:v>31.74148509320445</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>31.78091277594399</c:v>
+                  <c:v>31.91182445709946</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>32.72037620303544</c:v>
+                  <c:v>33.13543507821868</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>32.45405063508703</c:v>
+                  <c:v>32.47203807046262</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>32.33418207108352</c:v>
+                  <c:v>32.29163087609478</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>32.59138836830541</c:v>
+                  <c:v>32.68150552869755</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3797,6 +3823,1055 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2085087288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exponential Moving Average'!$A$3:$A$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="114"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>32.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>34.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>44.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>54.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>55.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>56.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>57.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>58.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>59.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>61.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>62.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>64.0</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>65.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>66.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>68.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>69.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>71.0</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>72.0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>73.0</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>75.0</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>76.0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>77.0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>78.0</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>79.0</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>80.0</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>81.0</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>83.0</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>84.0</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>85.0</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>86.0</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>87.0</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>88.0</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>89.0</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>90.0</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>92.0</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>94.0</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>95.0</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>96.0</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>97.0</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>98.0</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>99.0</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>101.0</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>102.0</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>103.0</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>104.0</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>105.0</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>106.0</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>107.0</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>108.0</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>109.0</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>110.0</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>111.0</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>112.0</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>113.0</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>114.0</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>115.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exponential Moving Average'!$E$3:$E$116</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="114"/>
+                <c:pt idx="0">
+                  <c:v>17.091154036195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.99282296297577</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.07116919477674</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.20534851780847</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.37364427362941</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.19583813535249</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.35971074457821</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.48341457262442</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>23.0928535533637</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.56564740375876</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.77361175257159</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.94014285176711</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.80974119806667</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.01642217894032</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.07115491110316</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.2390614912603</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.41377934455634</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>19.55592910111731</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19.94776885979135</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19.8484983612308</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>18.00688966370856</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.0613417697271</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.25640489136971</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.46996808774468</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>18.36695451500734</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>20.41081610624135</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>20.6399513027601</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>20.45311756238082</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>20.64097582207194</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>20.76508000701075</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>20.9888480188271</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>21.24808510459273</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>21.20006222453392</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>20.94740226439329</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>22.11715140452926</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>21.08875250064678</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>21.27198425302742</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>21.46477072872783</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>21.68782771677224</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>21.55970166447262</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>21.8826460632844</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>21.77027289091253</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>21.91717147319291</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>22.28475604858141</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>22.14116137761485</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>22.34070041275814</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>22.98788665442997</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>22.78837869268711</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>22.98464553755345</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>23.1584623498135</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>23.46785679876805</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>21.7257961629377</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>22.2514172094732</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>23.48263154566509</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>23.86597122764817</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>23.69510518133325</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>22.57982828541616</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>22.33962342475834</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>23.85299033090729</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>24.04080096515417</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>23.66081120782269</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>24.59391952450795</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>24.34803228187257</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>24.4983620472835</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>24.59573290052122</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>24.82765720777296</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>24.47636600558655</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>30.52266668893954</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>25.17290749770664</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>25.63389783523031</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>25.35486105110928</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>25.72608059103316</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>25.59048410097082</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>25.81013970373015</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>26.15461339845439</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>25.32897153905701</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>26.02587758108298</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>27.0322346837959</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>26.7878958290386</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>27.04953019854217</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>27.26060074609303</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>27.45624164775275</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>27.74652297873577</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>28.22580257746844</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>27.25701793135909</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>28.0115557625376</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>28.11682845097535</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>28.49778966091936</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>28.78451280164315</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>29.3930270797228</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>28.59923617284661</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>28.56501141476921</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>28.92537801665526</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>29.84144191276105</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>29.82988073273096</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>30.05196634702308</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>30.59780363181758</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>30.33375194561857</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>29.81024421167863</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>30.15462925781343</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>30.46928448548721</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>30.98295946315815</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>30.91762069141208</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>31.34695279757024</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>31.30084691426127</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>31.4085089050336</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>31.77109685006959</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>32.01976038990306</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>33.14140518260395</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>32.46524512088422</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>32.66773417595142</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>32.69727140770376</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2109500120"/>
+        <c:axId val="-2108766728"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2109500120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2108766728"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2108766728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2109500120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exponential Moving Average'!$A$7:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exponential Moving Average'!$H$7:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>18.21933531263316</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.09433912733036</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.30962919691046</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.39340185621226</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.39800619581176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>18.57759260633426</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>18.62516188123666</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.17463278272586</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.45273947217906</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>18.91662573316536</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>19.06867765882456</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>19.28092932203246</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>19.40253424146616</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.58084845045056</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.15903639295536</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.60449957349736</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>19.83502363660776</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>20.08192991712526</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20.14558958509406</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20.17629599073366</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20.16987394788696</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20.49151777723276</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>20.78413176038696</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>20.09415220716436</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>20.61700796583136</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2092988024"/>
+        <c:axId val="-2111756184"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2092988024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2111756184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2111756184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2092988024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3947,16 +5022,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>717550</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3970,6 +5045,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>577850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -13458,7 +14593,7 @@
   <dimension ref="A2:E183"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B116"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -15760,23 +16895,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E116"/>
+  <dimension ref="A1:H116"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:8">
       <c r="D1" t="s">
         <v>23</v>
       </c>
       <c r="E1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>0.7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -15787,8 +16928,11 @@
         <f>B2</f>
         <v>17.988252639770501</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
@@ -15797,10 +16941,18 @@
       </c>
       <c r="C3">
         <f>$E$1*B3+(1-$E$1)*C2</f>
-        <v>17.982629776000948</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>17.98038063049313</v>
+      </c>
+      <c r="D3">
+        <f>B3-B2</f>
+        <v>-1.124572753910158E-2</v>
+      </c>
+      <c r="E3">
+        <f>C3+$G$1/D3</f>
+        <v>17.091154036195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>3</v>
       </c>
@@ -15809,10 +16961,18 @@
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C67" si="0">$E$1*B4+(1-$E$1)*C3</f>
-        <v>17.984779357910124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>17.984964447021447</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D67" si="1">B4-B3</f>
+        <v>9.9220275879012831E-3</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E67" si="2">C4+$G$1/D4</f>
+        <v>18.992822962975765</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>4</v>
       </c>
@@ -15821,10 +16981,18 @@
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>17.990490913391064</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>17.992831062316831</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>9.2735290526988479E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>19.071169194776743</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>5</v>
       </c>
@@ -15833,10 +17001,25 @@
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>18.022993564605681</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>18.036696669769256</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>5.9293746948299031E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>18.205348517808467</v>
+      </c>
+      <c r="F6">
+        <v>-4.4019455699562116E-2</v>
+      </c>
+      <c r="H6">
+        <f>B6-F6</f>
+        <v>18.09951567151986</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>6</v>
       </c>
@@ -15845,10 +17028,25 @@
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>18.253882646560641</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>18.350349210891697</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.42927551269530184</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>18.373644273629406</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.26543641588244071</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H33" si="3">B7-F7</f>
+        <v>18.219335312633159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>7</v>
       </c>
@@ -15857,10 +17055,25 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>18.214873909950221</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>18.228210384605369</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>-0.30890655517579901</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>18.195838135352489</v>
+      </c>
+      <c r="F8" s="1">
+        <v>8.1526046009440023E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>18.094339127330361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>8</v>
       </c>
@@ -15869,10 +17082,25 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>18.261307537555659</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>18.283881930994383</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.13187599182129972</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>18.359710744578212</v>
+      </c>
+      <c r="F9" s="1">
+        <v>-1.8880317493596976E-3</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>18.309629196910461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>9</v>
       </c>
@@ -15881,10 +17109,25 @@
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>18.32351055741308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>18.355164083387667</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>7.7972412109399869E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>18.483414572624415</v>
+      </c>
+      <c r="F10" s="1">
+        <v>-7.6882789417602737E-3</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>18.393401856212261</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>10</v>
       </c>
@@ -15893,10 +17136,25 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>18.355672553181591</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>18.378033409281372</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.1209716795986822E-3</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>23.092853553363703</v>
+      </c>
+      <c r="F11" s="1">
+        <v>-1.0171646861660832E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>18.39800619581176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>11</v>
       </c>
@@ -15905,10 +17163,25 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>18.460718967020448</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>18.509445789385921</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>0.177930831909201</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="2"/>
+        <v>18.565647403758764</v>
+      </c>
+      <c r="F12" s="1">
+        <v>-1.1827225474959846E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>18.57759260633426</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>12</v>
       </c>
@@ -15917,10 +17190,25 @@
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>18.539925027638624</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>18.586225498595535</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>5.3365707397500017E-2</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>18.773611752571593</v>
+      </c>
+      <c r="F13" s="1">
+        <v>-6.0307929798604221E-3</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>18.625161881236661</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>13</v>
       </c>
@@ -15929,10 +17217,25 @@
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>18.79964848794036</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>18.917428013348129</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>0.44024085998529827</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>18.94014285176711</v>
+      </c>
+      <c r="F14" s="1">
+        <v>-0.11526083448375957</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="3"/>
+        <v>19.174632782725858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>14</v>
       </c>
@@ -15941,10 +17244,25 @@
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
-        <v>18.81201563496138</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>18.85229635139212</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>-0.23498916625969812</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>18.809741198066675</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.37164330980333915</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="3"/>
+        <v>18.452739472179061</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>15</v>
       </c>
@@ -15953,10 +17271,25 @@
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
-        <v>18.856752446386942</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
+        <v>18.886731385886385</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>7.7106475830099441E-2</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>19.016422178940324</v>
+      </c>
+      <c r="F16" s="1">
+        <v>-1.5136475352861112E-2</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="3"/>
+        <v>18.916625733165361</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -15965,10 +17298,25 @@
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
-        <v>18.958456064807223</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
+        <v>19.008131194025168</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>0.15867042541499998</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>19.071154911103164</v>
+      </c>
+      <c r="F17" s="1">
+        <v>-8.5179755970621329E-3</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="3"/>
+        <v>19.068677658824562</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -15977,10 +17325,25 @@
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
-        <v>19.114192975335712</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
+        <v>19.191390278312493</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>0.20977020263670099</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>19.239061491260305</v>
+      </c>
+      <c r="F18" s="1">
+        <v>-1.0999436168262378E-2</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="3"/>
+        <v>19.280929322032463</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -15989,10 +17352,25 @@
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
-        <v>19.253691679623408</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
+        <v>19.332650352231518</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>0.12326049804689987</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>19.413779344556335</v>
+      </c>
+      <c r="F19" s="1">
+        <v>-9.3438575550592873E-3</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="3"/>
+        <v>19.40253424146616</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -16001,10 +17379,25 @@
       </c>
       <c r="C20">
         <f t="shared" si="0"/>
-        <v>19.412598136259454</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
+        <v>19.499848320696305</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>0.17831420898439987</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="2"/>
+        <v>19.555929101117314</v>
+      </c>
+      <c r="F20" s="1">
+        <v>-9.3438575550592873E-3</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="3"/>
+        <v>19.58084845045056</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -16013,10 +17406,25 @@
       </c>
       <c r="C21">
         <f t="shared" si="0"/>
-        <v>19.762984515822577</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+        <v>19.92931412297888</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>0.54186630249019885</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="2"/>
+        <v>19.947768859791346</v>
+      </c>
+      <c r="F21" s="1">
+        <v>-4.566549756966154E-2</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="3"/>
+        <v>20.159036392955361</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -16025,10 +17433,25 @@
       </c>
       <c r="C22">
         <f t="shared" si="0"/>
-        <v>19.818188310462538</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
+        <v>19.890168710465414</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>-0.23997879028319957</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="2"/>
+        <v>19.848498361230803</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0.2688925316051396</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="3"/>
+        <v>19.60449957349736</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -16037,10 +17460,25 @@
       </c>
       <c r="C23">
         <f t="shared" si="0"/>
-        <v>19.843113243976369</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
+        <v>19.874677337382764</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>-5.3539276123011348E-3</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="2"/>
+        <v>18.006889663708563</v>
+      </c>
+      <c r="F23" s="1">
+        <v>3.3014540882440713E-2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="3"/>
+        <v>19.835023636607758</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -16049,10 +17487,25 @@
       </c>
       <c r="C24">
         <f t="shared" si="0"/>
-        <v>19.957021862466682</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
+        <v>20.01205453788473</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>0.20289230346680043</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="2"/>
+        <v>20.061341769727097</v>
+      </c>
+      <c r="F24" s="1">
+        <v>-1.0999436168262378E-2</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>20.081929917125262</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -16061,10 +17514,25 @@
       </c>
       <c r="C25">
         <f t="shared" si="0"/>
-        <v>20.045392111042894</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
+        <v>20.09725001309879</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>6.283187866210227E-2</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="2"/>
+        <v>20.256404891369709</v>
+      </c>
+      <c r="F25" s="1">
+        <v>-1.1827225474959846E-2</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="3"/>
+        <v>20.145589585094061</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -16073,10 +17541,25 @@
       </c>
       <c r="C26">
         <f t="shared" si="0"/>
-        <v>20.104930438150795</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
+        <v>20.144303139610727</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>3.07064056395987E-2</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="2"/>
+        <v>20.469968087744679</v>
+      </c>
+      <c r="F26" s="1">
+        <v>-1.1827225474959846E-2</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="3"/>
+        <v>20.17629599073366</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>26</v>
       </c>
@@ -16085,10 +17568,25 @@
       </c>
       <c r="C27">
         <f t="shared" si="0"/>
-        <v>20.131902474934748</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
+        <v>20.154503100086309</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>-5.5942535399999826E-3</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="2"/>
+        <v>18.366954515007336</v>
+      </c>
+      <c r="F27" s="1">
+        <v>-1.0999436168262378E-2</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="3"/>
+        <v>20.169873947886963</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>27</v>
       </c>
@@ -16097,10 +17595,25 @@
       </c>
       <c r="C28">
         <f t="shared" si="0"/>
-        <v>20.303727993753974</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
+        <v>20.379238388827133</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>0.31667900085449929</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="2"/>
+        <v>20.410816106241349</v>
+      </c>
+      <c r="F28" s="1">
+        <v>-1.5964264659562133E-2</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="3"/>
+        <v>20.491517777232762</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>28</v>
       </c>
@@ -16109,10 +17622,25 @@
       </c>
       <c r="C29">
         <f t="shared" si="0"/>
-        <v>20.493229811085939</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
+        <v>20.59168365654067</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>0.20717811584470169</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="2"/>
+        <v>20.6399513027601</v>
+      </c>
+      <c r="F29" s="1">
+        <v>-0.10140013196906139</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="3"/>
+        <v>20.784131760386963</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>29</v>
       </c>
@@ -16121,10 +17649,25 @@
       </c>
       <c r="C30">
         <f t="shared" si="0"/>
-        <v>20.47512766952002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
+        <v>20.497422966530074</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>-0.22570610046379969</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="2"/>
+        <v>20.453117562380822</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0.36287332078973833</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="3"/>
+        <v>20.094152207164363</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>30</v>
       </c>
@@ -16133,10 +17676,25 @@
       </c>
       <c r="C31">
         <f t="shared" si="0"/>
-        <v>20.541395888898158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
+        <v>20.574591765752434</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>0.15063858032219812</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="2"/>
+        <v>20.640975822071944</v>
+      </c>
+      <c r="F31" s="1">
+        <v>-9.3438575550592873E-3</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="3"/>
+        <v>20.617007965831359</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>31</v>
       </c>
@@ -16145,10 +17703,25 @@
       </c>
       <c r="C32">
         <f t="shared" si="0"/>
-        <v>20.634782188223479</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
+        <v>20.682095471009887</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>0.12050437927250002</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="2"/>
+        <v>20.765080007010749</v>
+      </c>
+      <c r="F32" s="1">
+        <v>-1.1827225474959846E-2</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="3"/>
+        <v>20.73999571302376</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>32</v>
       </c>
@@ -16157,10 +17730,25 @@
       </c>
       <c r="C33">
         <f t="shared" si="0"/>
-        <v>20.70179623022009</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
+        <v>20.742795831854657</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>4.0641784667901248E-2</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="2"/>
+        <v>20.988848018827095</v>
+      </c>
+      <c r="F33" s="1">
+        <v>-1.1827225474959846E-2</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="3"/>
+        <v>20.780637497691661</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>33</v>
       </c>
@@ -16169,10 +17757,25 @@
       </c>
       <c r="C34">
         <f t="shared" si="0"/>
-        <v>20.735303251218397</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
+        <v>20.761005940108088</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E34" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F34" s="1">
+        <v>-1.2655014781561391E-2</v>
+      </c>
+      <c r="H34">
+        <f>B34-F34</f>
+        <v>20.781465286998262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>34</v>
       </c>
@@ -16181,10 +17784,19 @@
       </c>
       <c r="C35">
         <f t="shared" si="0"/>
-        <v>20.762772246336699</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
+        <v>20.781470651050928</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="1"/>
+        <v>2.1430969238299014E-2</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="2"/>
+        <v>21.248085104592725</v>
+      </c>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>35</v>
       </c>
@@ -16193,10 +17805,18 @@
       </c>
       <c r="C36">
         <f t="shared" si="0"/>
-        <v>21.058448157775249</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
+        <v>21.18232804376494</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="1"/>
+        <v>0.56388282775879972</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="2"/>
+        <v>21.200062224533923</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
@@ -16205,10 +17825,18 @@
       </c>
       <c r="C37">
         <f t="shared" si="0"/>
-        <v>20.967543285125373</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
+        <v>20.968345301862332</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="1"/>
+        <v>-0.47748565673829901</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="2"/>
+        <v>20.94740226439329</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
@@ -16217,10 +17845,18 @@
       </c>
       <c r="C38">
         <f t="shared" si="0"/>
-        <v>20.926232656356586</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
+        <v>20.909949009870157</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="1"/>
+        <v>8.2836151122975821E-3</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="2"/>
+        <v>22.117151404529263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>38</v>
       </c>
@@ -16229,10 +17865,18 @@
       </c>
       <c r="C39">
         <f t="shared" si="0"/>
-        <v>20.90557734197219</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
+        <v>20.892430122272504</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>39</v>
       </c>
@@ -16241,10 +17885,18 @@
       </c>
       <c r="C40">
         <f t="shared" si="0"/>
-        <v>21.007384618251695</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
+        <v>21.044163362853592</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="1"/>
+        <v>0.22426986694340201</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="2"/>
+        <v>21.088752500646784</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>40</v>
       </c>
@@ -16253,10 +17905,18 @@
       </c>
       <c r="C41">
         <f t="shared" si="0"/>
-        <v>21.097558657392447</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
+        <v>21.144661896429316</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="1"/>
+        <v>7.854080200199931E-2</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="2"/>
+        <v>21.271984253027423</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>41</v>
       </c>
@@ -16265,10 +17925,18 @@
       </c>
       <c r="C42">
         <f t="shared" si="0"/>
-        <v>21.161629517905176</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
+        <v>21.201388833821326</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="1"/>
+        <v>3.7967681884701676E-2</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="2"/>
+        <v>21.464770728727828</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>42</v>
       </c>
@@ -16277,10 +17945,18 @@
       </c>
       <c r="C43">
         <f t="shared" si="0"/>
-        <v>21.517952362712336</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
+        <v>21.672409295410048</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="1"/>
+        <v>0.64857482910159803</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="2"/>
+        <v>21.68782771677224</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>43</v>
       </c>
@@ -16289,10 +17965,18 @@
       </c>
       <c r="C44">
         <f t="shared" si="0"/>
-        <v>21.537141044942565</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
+        <v>21.591153597643974</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="1"/>
+        <v>-0.317945480346701</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="2"/>
+        <v>21.559701664472616</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>44</v>
       </c>
@@ -16301,10 +17985,18 @@
       </c>
       <c r="C45">
         <f t="shared" si="0"/>
-        <v>21.563865284128983</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3">
+        <v>21.590758745613975</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="1"/>
+        <v>3.4259796142602994E-2</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="2"/>
+        <v>21.882646063284401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>45</v>
       </c>
@@ -16313,10 +18005,18 @@
       </c>
       <c r="C46">
         <f t="shared" si="0"/>
-        <v>21.664713670812041</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3">
+        <v>21.713121063930764</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="1"/>
+        <v>0.17497253417969816</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="2"/>
+        <v>21.770272890912533</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -16325,10 +18025,18 @@
       </c>
       <c r="C47">
         <f t="shared" si="0"/>
-        <v>21.77425899605052</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>21.83259934408153</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="1"/>
+        <v>0.11824226379389913</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="2"/>
+        <v>21.917171473192912</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>47</v>
       </c>
@@ -16337,10 +18045,18 @@
       </c>
       <c r="C48">
         <f t="shared" si="0"/>
-        <v>21.841570568581858</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>21.885997302003698</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="1"/>
+        <v>2.5077819824200986E-2</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="2"/>
+        <v>22.284756048581407</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49">
         <v>48</v>
       </c>
@@ -16349,10 +18065,18 @@
       </c>
       <c r="C49">
         <f t="shared" si="0"/>
-        <v>22.021653509388578</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>22.107014705737818</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="1"/>
+        <v>0.29285430908209875</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="2"/>
+        <v>22.141161377614846</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50">
         <v>49</v>
       </c>
@@ -16361,10 +18085,18 @@
       </c>
       <c r="C50">
         <f t="shared" si="0"/>
-        <v>22.170035052423739</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>22.254996028542575</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="1"/>
+        <v>0.11668014526360082</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="2"/>
+        <v>22.340700412758142</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51">
         <v>50</v>
       </c>
@@ -16373,10 +18105,18 @@
       </c>
       <c r="C51">
         <f t="shared" si="0"/>
-        <v>22.72863610989107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3">
+        <v>22.97756482571365</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="1"/>
+        <v>0.96882057189949933</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="2"/>
+        <v>22.987886654429975</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52">
         <v>51</v>
       </c>
@@ -16385,10 +18125,18 @@
       </c>
       <c r="C52">
         <f t="shared" si="0"/>
-        <v>22.730857056410336</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
+        <v>22.806424049764814</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="1"/>
+        <v>-0.55415916442879976</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="2"/>
+        <v>22.788378692687111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53">
         <v>52</v>
       </c>
@@ -16397,10 +18145,18 @@
       </c>
       <c r="C53">
         <f t="shared" si="0"/>
-        <v>22.870083412543519</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3">
+        <v>22.948444053003136</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="1"/>
+        <v>0.27623176574710229</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="2"/>
+        <v>22.984645537553451</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54">
         <v>53</v>
       </c>
@@ -16409,10 +18165,18 @@
       </c>
       <c r="C54">
         <f t="shared" si="0"/>
-        <v>22.997635166354762</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3">
+        <v>23.07216406001714</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="1"/>
+        <v>0.11587715148930045</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="2"/>
+        <v>23.158462349813497</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55">
         <v>54</v>
       </c>
@@ -16421,10 +18185,18 @@
       </c>
       <c r="C55">
         <f t="shared" si="0"/>
-        <v>23.076210161302381</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3">
+        <v>23.129998827380142</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="1"/>
+        <v>2.9598236083998586E-2</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="2"/>
+        <v>23.467856798768047</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56">
         <v>55</v>
       </c>
@@ -16433,10 +18205,18 @@
       </c>
       <c r="C56">
         <f t="shared" si="0"/>
-        <v>23.111968110131141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3">
+        <v>23.142407889485973</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="1"/>
+        <v>-7.0590972900994586E-3</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="2"/>
+        <v>21.725796162937705</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57">
         <v>56</v>
       </c>
@@ -16445,10 +18225,18 @@
       </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>23.12420896198692</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
+        <v>23.13823723653568</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="1"/>
+        <v>-1.1276245117201711E-2</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="2"/>
+        <v>22.2514172094732</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58">
         <v>57</v>
       </c>
@@ -16457,10 +18245,18 @@
       </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>23.361789005529559</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3">
+        <v>23.461029505311245</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="1"/>
+        <v>0.46291923522950285</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="2"/>
+        <v>23.482631545665093</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59">
         <v>58</v>
       </c>
@@ -16469,10 +18265,18 @@
       </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>23.683010706072878</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3">
+        <v>23.841271536224713</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="1"/>
+        <v>0.4048633575439986</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="2"/>
+        <v>23.865971227648167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60">
         <v>59</v>
       </c>
@@ -16481,10 +18285,18 @@
       </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>23.679497067513939</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
+        <v>23.725569861135916</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="1"/>
+        <v>-0.32824897766120031</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="2"/>
+        <v>23.695105181333254</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61">
         <v>60</v>
       </c>
@@ -16493,10 +18305,18 @@
       </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>23.673214109928821</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3">
+        <v>23.684522764981367</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="1"/>
+        <v>-9.0522766112997033E-3</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="2"/>
+        <v>22.579828285416163</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62">
         <v>61</v>
       </c>
@@ -16505,10 +18325,18 @@
       </c>
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>23.66630561758646</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3">
+        <v>23.666934817165281</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="1"/>
+        <v>-7.5340270995987169E-3</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="2"/>
+        <v>22.33962342475834</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63">
         <v>62</v>
       </c>
@@ -16517,10 +18345,18 @@
       </c>
       <c r="C63">
         <f t="shared" si="0"/>
-        <v>23.76431945765793</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3">
+        <v>23.803713753560167</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="1"/>
+        <v>0.20293617248529827</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="2"/>
+        <v>23.852990330907286</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64">
         <v>63</v>
       </c>
@@ -16529,10 +18365,18 @@
       </c>
       <c r="C64">
         <f t="shared" si="0"/>
-        <v>23.919831771675614</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3">
+        <v>23.993854986053357</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="1"/>
+        <v>0.21301078796389916</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="2"/>
+        <v>24.040800965154165</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65">
         <v>64</v>
       </c>
@@ -16541,10 +18385,18 @@
       </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>23.984119186313855</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
+        <v>24.032041116482475</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="1"/>
+        <v>-2.6937484741200279E-2</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="2"/>
+        <v>23.660811207822693</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66">
         <v>65</v>
       </c>
@@ -16553,10 +18405,18 @@
       </c>
       <c r="C66">
         <f t="shared" si="0"/>
-        <v>24.400117759660827</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3">
+        <v>24.580893768050203</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="1"/>
+        <v>0.76770973205569959</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="2"/>
+        <v>24.59391952450795</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67">
         <v>66</v>
       </c>
@@ -16565,10 +18425,18 @@
       </c>
       <c r="C67">
         <f t="shared" si="0"/>
-        <v>24.337367000557911</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3">
+        <v>24.366499499433559</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="1"/>
+        <v>-0.54150009155279832</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="2"/>
+        <v>24.348032281872573</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68">
         <v>67</v>
       </c>
@@ -16576,11 +18444,19 @@
         <v>24.341598510742099</v>
       </c>
       <c r="C68">
-        <f t="shared" ref="C68:C116" si="1">$E$1*B68+(1-$E$1)*C67</f>
-        <v>24.339482755650003</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
+        <f t="shared" ref="C68:C116" si="4">$E$1*B68+(1-$E$1)*C67</f>
+        <v>24.349068807349536</v>
+      </c>
+      <c r="D68">
+        <f t="shared" ref="D68:D116" si="5">B68-B67</f>
+        <v>6.6982269287098717E-2</v>
+      </c>
+      <c r="E68">
+        <f t="shared" ref="E68:E116" si="6">C68+$G$1/D68</f>
+        <v>24.498362047283496</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69">
         <v>68</v>
       </c>
@@ -16588,11 +18464,19 @@
         <v>24.656009674072202</v>
       </c>
       <c r="C69">
-        <f t="shared" si="1"/>
-        <v>24.497746214861102</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>24.563927414055399</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="5"/>
+        <v>0.31441116333010299</v>
+      </c>
+      <c r="E69">
+        <f t="shared" si="6"/>
+        <v>24.595732900521224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70">
         <v>69</v>
       </c>
@@ -16600,11 +18484,19 @@
         <v>24.721054077148398</v>
       </c>
       <c r="C70">
-        <f t="shared" si="1"/>
-        <v>24.609400146004752</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>24.6739160782205</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="5"/>
+        <v>6.5044403076196744E-2</v>
+      </c>
+      <c r="E70">
+        <f t="shared" si="6"/>
+        <v>24.827657207772962</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71">
         <v>70</v>
       </c>
@@ -16612,11 +18504,19 @@
         <v>24.669658660888601</v>
       </c>
       <c r="C71">
-        <f t="shared" si="1"/>
-        <v>24.639529403446677</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>24.67093588608817</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="5"/>
+        <v>-5.1395416259797599E-2</v>
+      </c>
+      <c r="E71">
+        <f t="shared" si="6"/>
+        <v>24.476366005586545</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72">
         <v>71</v>
       </c>
@@ -16624,11 +18524,19 @@
         <v>24.671367645263601</v>
       </c>
       <c r="C72">
-        <f t="shared" si="1"/>
-        <v>24.655448524355137</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>24.671238117510971</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="5"/>
+        <v>1.708984375E-3</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="6"/>
+        <v>30.522666688939541</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73">
         <v>72</v>
       </c>
@@ -16636,11 +18544,19 @@
         <v>24.6918926239013</v>
       </c>
       <c r="C73">
-        <f t="shared" si="1"/>
-        <v>24.673670574128217</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>24.685696271984202</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="5"/>
+        <v>2.0524978637698865E-2</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="6"/>
+        <v>25.172907497706635</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74">
         <v>73</v>
       </c>
@@ -16648,11 +18564,19 @@
         <v>26.0295906066894</v>
       </c>
       <c r="C74">
-        <f t="shared" si="1"/>
-        <v>25.35163059040881</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.626422306277838</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="5"/>
+        <v>1.3376979827881001</v>
+      </c>
+      <c r="E74">
+        <f t="shared" si="6"/>
+        <v>25.633897835230314</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75">
         <v>74</v>
       </c>
@@ -16660,11 +18584,19 @@
         <v>25.2569675445556</v>
       </c>
       <c r="C75">
-        <f t="shared" si="1"/>
-        <v>25.304299067482205</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.36780397307227</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="5"/>
+        <v>-0.77262306213379972</v>
+      </c>
+      <c r="E75">
+        <f t="shared" si="6"/>
+        <v>25.354861051109285</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76">
         <v>75</v>
       </c>
@@ -16672,11 +18604,19 @@
         <v>25.280824661254801</v>
       </c>
       <c r="C76">
-        <f t="shared" si="1"/>
-        <v>25.292561864368501</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.306918454800041</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="5"/>
+        <v>2.3857116699200986E-2</v>
+      </c>
+      <c r="E76">
+        <f t="shared" si="6"/>
+        <v>25.726080591033163</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77">
         <v>76</v>
       </c>
@@ -16684,11 +18624,19 @@
         <v>25.675848007202099</v>
       </c>
       <c r="C77">
-        <f t="shared" si="1"/>
-        <v>25.4842049357853</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.56516914148148</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="5"/>
+        <v>0.3950233459472976</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="6"/>
+        <v>25.590484100970823</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78">
         <v>77</v>
       </c>
@@ -16696,11 +18644,19 @@
         <v>25.790205001831001</v>
       </c>
       <c r="C78">
-        <f t="shared" si="1"/>
-        <v>25.637204968808149</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.722694243726146</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="5"/>
+        <v>0.1143569946289027</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="6"/>
+        <v>25.810139703730151</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79">
         <v>78</v>
       </c>
@@ -16708,11 +18664,19 @@
         <v>25.817564010620099</v>
       </c>
       <c r="C79">
-        <f t="shared" si="1"/>
-        <v>25.727384489714126</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.789103080551914</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="5"/>
+        <v>2.7359008789098027E-2</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="6"/>
+        <v>26.154613398454394</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80">
         <v>79</v>
       </c>
@@ -16720,11 +18684,19 @@
         <v>25.796058654785099</v>
       </c>
       <c r="C80">
-        <f t="shared" si="1"/>
-        <v>25.761721572249613</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.793971982515146</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="5"/>
+        <v>-2.1505355835000017E-2</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="6"/>
+        <v>25.328971539057012</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81">
         <v>80</v>
       </c>
@@ -16732,11 +18704,19 @@
         <v>26.073837280273398</v>
       </c>
       <c r="C81">
-        <f t="shared" si="1"/>
-        <v>25.917779426261504</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>25.989877690945924</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="5"/>
+        <v>0.27777862548829901</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="6"/>
+        <v>26.025877581082977</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82">
         <v>81</v>
       </c>
@@ -16744,11 +18724,19 @@
         <v>27.4687175750732</v>
       </c>
       <c r="C82">
-        <f t="shared" si="1"/>
-        <v>26.693248500667352</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.025065609835018</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="5"/>
+        <v>1.3948802947998011</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="6"/>
+        <v>27.032234683795902</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83">
         <v>82</v>
       </c>
@@ -16756,11 +18744,19 @@
         <v>26.7049560546875</v>
       </c>
       <c r="C83">
-        <f t="shared" si="1"/>
-        <v>26.699102277677426</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>26.800988921231756</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="5"/>
+        <v>-0.76376152038569955</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="6"/>
+        <v>26.787895829038593</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84">
         <v>83</v>
       </c>
@@ -16768,11 +18764,19 @@
         <v>27.1217746734619</v>
       </c>
       <c r="C84">
-        <f t="shared" si="1"/>
-        <v>26.910438475569663</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.025538947792853</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="5"/>
+        <v>0.41681861877439985</v>
+      </c>
+      <c r="E84">
+        <f t="shared" si="6"/>
+        <v>27.049530198542168</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85">
         <v>84</v>
       </c>
@@ -16780,11 +18784,19 @@
         <v>27.2336616516113</v>
       </c>
       <c r="C85">
-        <f t="shared" si="1"/>
-        <v>27.072050063590481</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.171224840465769</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="5"/>
+        <v>0.11188697814939985</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="6"/>
+        <v>27.260600746093029</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86">
         <v>85</v>
       </c>
@@ -16792,11 +18804,19 @@
         <v>27.5302200317382</v>
       </c>
       <c r="C86">
-        <f t="shared" si="1"/>
-        <v>27.301135047664339</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.422521474356472</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="5"/>
+        <v>0.29655838012689983</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="6"/>
+        <v>27.456241647752755</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87">
         <v>86</v>
       </c>
@@ -16804,11 +18824,19 @@
         <v>27.839136123657202</v>
       </c>
       <c r="C87">
-        <f t="shared" si="1"/>
-        <v>27.570135585660772</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.714151728866984</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="5"/>
+        <v>0.30891609191900216</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="6"/>
+        <v>27.746522978735772</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88">
         <v>87</v>
       </c>
@@ -16816,11 +18844,19 @@
         <v>27.8637084960937</v>
       </c>
       <c r="C88">
-        <f t="shared" si="1"/>
-        <v>27.716922040877236</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.818841465925686</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="5"/>
+        <v>2.4572372436498569E-2</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="6"/>
+        <v>28.225802577468443</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89">
         <v>88</v>
       </c>
@@ -16828,11 +18864,19 @@
         <v>27.846502304077099</v>
       </c>
       <c r="C89">
-        <f t="shared" si="1"/>
-        <v>27.781712172477167</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.838204052631674</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="5"/>
+        <v>-1.7206192016601562E-2</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="6"/>
+        <v>27.257017931359087</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90">
         <v>89</v>
       </c>
@@ -16840,11 +18884,19 @@
         <v>27.9601726531982</v>
       </c>
       <c r="C90">
-        <f t="shared" si="1"/>
-        <v>27.870942412837685</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>27.923582073028243</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="5"/>
+        <v>0.11367034912110086</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="6"/>
+        <v>28.011555762537601</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91">
         <v>90</v>
       </c>
@@ -16852,11 +18904,19 @@
         <v>28.072738647460898</v>
       </c>
       <c r="C91">
-        <f t="shared" si="1"/>
-        <v>27.971840530149294</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.027991675131101</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="5"/>
+        <v>0.11256599426269887</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="6"/>
+        <v>28.116828450975348</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92">
         <v>91</v>
       </c>
@@ -16864,11 +18924,19 @@
         <v>28.675428390502901</v>
       </c>
       <c r="C92">
-        <f t="shared" si="1"/>
-        <v>28.323634460326097</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.481197375891362</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="5"/>
+        <v>0.60268974304200285</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="6"/>
+        <v>28.497789660919356</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93">
         <v>92</v>
       </c>
@@ -16876,11 +18944,19 @@
         <v>28.796892166137599</v>
       </c>
       <c r="C93">
-        <f t="shared" si="1"/>
-        <v>28.56026331323185</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.70218372906373</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="5"/>
+        <v>0.12146377563469812</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="6"/>
+        <v>28.784512801643153</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94">
         <v>93</v>
       </c>
@@ -16888,11 +18964,19 @@
         <v>28.8132019042968</v>
       </c>
       <c r="C94">
-        <f t="shared" si="1"/>
-        <v>28.686732608764324</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.779896451726877</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="5"/>
+        <v>1.6309738159201004E-2</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="6"/>
+        <v>29.393027079722803</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95">
         <v>94</v>
       </c>
@@ -16900,11 +18984,19 @@
         <v>28.7508220672607</v>
       </c>
       <c r="C95">
-        <f t="shared" si="1"/>
-        <v>28.718777338012512</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.759544382600552</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="5"/>
+        <v>-6.2379837036100838E-2</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="6"/>
+        <v>28.599236172846609</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96">
         <v>95</v>
       </c>
@@ -16912,11 +19004,19 @@
         <v>28.6781101226806</v>
       </c>
       <c r="C96">
-        <f t="shared" si="1"/>
-        <v>28.698443730346554</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.702540400656588</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="5"/>
+        <v>-7.2711944580099441E-2</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="6"/>
+        <v>28.565011414769213</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97">
         <v>96</v>
       </c>
@@ -16924,11 +19024,19 @@
         <v>28.972324371337798</v>
       </c>
       <c r="C97">
-        <f t="shared" si="1"/>
-        <v>28.835384050842176</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>28.891389180133434</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="5"/>
+        <v>0.29421424865719814</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="6"/>
+        <v>28.925378016655255</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98">
         <v>97</v>
       </c>
@@ -16936,11 +19044,19 @@
         <v>30.2373142242431</v>
       </c>
       <c r="C98">
-        <f t="shared" si="1"/>
-        <v>29.536349137542636</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.833536711010197</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="5"/>
+        <v>1.2649898529053019</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="6"/>
+        <v>29.841441912761052</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99">
         <v>98</v>
       </c>
@@ -16948,11 +19064,19 @@
         <v>29.866878509521399</v>
       </c>
       <c r="C99">
-        <f t="shared" si="1"/>
-        <v>29.701613823532018</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.856875969968037</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="5"/>
+        <v>-0.370435714721701</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="6"/>
+        <v>29.829880732730956</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100">
         <v>99</v>
       </c>
@@ -16960,11 +19084,19 @@
         <v>29.939876556396399</v>
       </c>
       <c r="C100">
-        <f t="shared" si="1"/>
-        <v>29.820745189964207</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.914976380467891</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="5"/>
+        <v>7.2998046875E-2</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="6"/>
+        <v>30.051966347023075</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101">
         <v>100</v>
       </c>
@@ -16972,11 +19104,19 @@
         <v>29.955150604248001</v>
       </c>
       <c r="C101">
-        <f t="shared" si="1"/>
-        <v>29.887947897106102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.943098337113966</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="5"/>
+        <v>1.527404785160158E-2</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="6"/>
+        <v>30.597803631817584</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102">
         <v>101</v>
       </c>
@@ -16984,11 +19124,19 @@
         <v>29.982704162597599</v>
       </c>
       <c r="C102">
-        <f t="shared" si="1"/>
-        <v>29.935326029851851</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.970822414952508</v>
+      </c>
+      <c r="D102">
+        <f t="shared" si="5"/>
+        <v>2.7553558349598717E-2</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="6"/>
+        <v>30.333751945618577</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103">
         <v>102</v>
       </c>
@@ -16996,11 +19144,19 @@
         <v>29.845687866210898</v>
       </c>
       <c r="C103">
-        <f t="shared" si="1"/>
-        <v>29.890506948031373</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>29.883228230833382</v>
+      </c>
+      <c r="D103">
+        <f t="shared" si="5"/>
+        <v>-0.13701629638670099</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="6"/>
+        <v>29.810244211678629</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104">
         <v>103</v>
       </c>
@@ -17008,11 +19164,19 @@
         <v>30.2341709136962</v>
       </c>
       <c r="C104">
-        <f t="shared" si="1"/>
-        <v>30.062338930863788</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>30.128888108837351</v>
+      </c>
+      <c r="D104">
+        <f t="shared" si="5"/>
+        <v>0.38848304748530182</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="6"/>
+        <v>30.154629257813429</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105">
         <v>104</v>
       </c>
@@ -17020,11 +19184,19 @@
         <v>30.5730075836181</v>
       </c>
       <c r="C105">
-        <f t="shared" si="1"/>
-        <v>30.317673257240944</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>30.439771741183876</v>
+      </c>
+      <c r="D105">
+        <f t="shared" si="5"/>
+        <v>0.33883666992189987</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="6"/>
+        <v>30.469284485487215</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106">
         <v>105</v>
       </c>
@@ -17032,11 +19204,19 @@
         <v>31.192701339721602</v>
       </c>
       <c r="C106">
-        <f t="shared" si="1"/>
-        <v>30.755187298481275</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>30.966822460160284</v>
+      </c>
+      <c r="D106">
+        <f t="shared" si="5"/>
+        <v>0.61969375610350141</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="6"/>
+        <v>30.982959463158149</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107">
         <v>106</v>
       </c>
@@ -17044,11 +19224,19 @@
         <v>30.9571933746337</v>
       </c>
       <c r="C107">
-        <f t="shared" si="1"/>
-        <v>30.856190336557489</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>30.960082100291675</v>
+      </c>
+      <c r="D107">
+        <f t="shared" si="5"/>
+        <v>-0.23550796508790128</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="6"/>
+        <v>30.917620691412075</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108">
         <v>107</v>
       </c>
@@ -17056,11 +19244,19 @@
         <v>30.9842224121093</v>
       </c>
       <c r="C108">
-        <f t="shared" si="1"/>
-        <v>30.920206374333397</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>30.97698031856401</v>
+      </c>
+      <c r="D108">
+        <f t="shared" si="5"/>
+        <v>2.7029037475600148E-2</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="6"/>
+        <v>31.346952797570236</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109">
         <v>108</v>
       </c>
@@ -17068,11 +19264,19 @@
         <v>31.018112182617099</v>
       </c>
       <c r="C109">
-        <f t="shared" si="1"/>
-        <v>30.969159278475246</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>31.005772623401171</v>
+      </c>
+      <c r="D109">
+        <f t="shared" si="5"/>
+        <v>3.3889770507798289E-2</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="6"/>
+        <v>31.300846914261268</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110">
         <v>109</v>
       </c>
@@ -17080,11 +19284,19 @@
         <v>31.554475784301701</v>
       </c>
       <c r="C110">
-        <f t="shared" si="1"/>
-        <v>31.261817531388473</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>31.389864836031542</v>
+      </c>
+      <c r="D110">
+        <f t="shared" si="5"/>
+        <v>0.53636360168460229</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="6"/>
+        <v>31.408508905033599</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111">
         <v>110</v>
       </c>
@@ -17092,11 +19304,19 @@
         <v>31.8921794891357</v>
       </c>
       <c r="C111">
-        <f t="shared" si="1"/>
-        <v>31.576998510262086</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>31.741485093204453</v>
+      </c>
+      <c r="D111">
+        <f t="shared" si="5"/>
+        <v>0.33770370483399859</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="6"/>
+        <v>31.77109685006959</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5">
       <c r="A112">
         <v>111</v>
       </c>
@@ -17104,11 +19324,19 @@
         <v>31.984827041625898</v>
       </c>
       <c r="C112">
-        <f t="shared" si="1"/>
-        <v>31.780912775943992</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>31.911824457099467</v>
+      </c>
+      <c r="D112">
+        <f t="shared" si="5"/>
+        <v>9.2647552490198848E-2</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="6"/>
+        <v>32.019760389903063</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113">
         <v>112</v>
       </c>
@@ -17116,11 +19344,19 @@
         <v>33.659839630126903</v>
       </c>
       <c r="C113">
-        <f t="shared" si="1"/>
-        <v>32.72037620303545</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>33.135435078218677</v>
+      </c>
+      <c r="D113">
+        <f t="shared" si="5"/>
+        <v>1.675012588501005</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="6"/>
+        <v>33.141405182603954</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114">
         <v>113</v>
       </c>
@@ -17128,11 +19364,19 @@
         <v>32.187725067138601</v>
       </c>
       <c r="C114">
-        <f t="shared" si="1"/>
-        <v>32.454050635087029</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>32.472038070462624</v>
+      </c>
+      <c r="D114">
+        <f t="shared" si="5"/>
+        <v>-1.4721145629883026</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="6"/>
+        <v>32.465245120884227</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115">
         <v>114</v>
       </c>
@@ -17140,11 +19384,19 @@
         <v>32.21431350708</v>
       </c>
       <c r="C115">
-        <f t="shared" si="1"/>
-        <v>32.334182071083518</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3">
+        <f t="shared" si="4"/>
+        <v>32.291630876094786</v>
+      </c>
+      <c r="D115">
+        <f t="shared" si="5"/>
+        <v>2.6588439941399145E-2</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="6"/>
+        <v>32.667734175951416</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116">
         <v>115</v>
       </c>
@@ -17152,12 +19404,21 @@
         <v>32.848594665527301</v>
       </c>
       <c r="C116">
-        <f t="shared" si="1"/>
-        <v>32.59138836830541</v>
+        <f t="shared" si="4"/>
+        <v>32.681505528697549</v>
+      </c>
+      <c r="D116">
+        <f t="shared" si="5"/>
+        <v>0.63428115844730115</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="6"/>
+        <v>32.697271407703759</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>